<commit_message>
Application Checklist: Requirements Specification
</commit_message>
<xml_diff>
--- a/Etapa 2/Checklist Gerência de Requisitos.xlsx
+++ b/Etapa 2/Checklist Gerência de Requisitos.xlsx
@@ -872,7 +872,7 @@
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="C3:C6 C20"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -989,7 +989,7 @@
   <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="B30" colorId="64" zoomScale="90" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C65" activeCellId="1" sqref="C3:C6 C65"/>
+      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="1" sqref="C3:C6 C13"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1955,7 +1955,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="1" sqref="C3:C6 H30"/>
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2064,7 +2064,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="1" sqref="C3:C6 C35"/>
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2154,7 +2154,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="1" sqref="C3:C6 C29"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2245,7 +2245,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C3:C6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2348,7 +2348,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H32" activeCellId="1" sqref="C3:C6 H32"/>
+      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2466,7 +2466,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>